<commit_message>
Fix apply_defaults for biquad modules
</commit_message>
<xml_diff>
--- a/fpga/pt_feedback/docs/pt_feedback_addresses.xlsx
+++ b/fpga/pt_feedback/docs/pt_feedback_addresses.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/polybox/ETHZ/Programming/Python/rp_interface/fpga/pt_feedback/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7629E5FC-4104-7449-86E8-2A01D529E3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A50094-F0CF-6E47-91AF-831567F1EE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6460" yWindow="-20480" windowWidth="28040" windowHeight="16940" xr2:uid="{6316E74E-F60B-2E49-B41A-03A0EDA0FE20}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6316E74E-F60B-2E49-B41A-03A0EDA0FE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
   <si>
     <t>GPIO Number</t>
   </si>
@@ -194,6 +194,15 @@
   </si>
   <si>
     <t>biquad_0-3, dc_block</t>
+  </si>
+  <si>
+    <t>pre-amp</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>trig mode</t>
   </si>
 </sst>
 </file>
@@ -597,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F040AB9C-6680-4A48-BD82-AA442C9BC840}">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,7 +878,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -885,7 +894,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -901,7 +910,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -917,7 +926,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -933,7 +942,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -949,7 +958,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -965,19 +974,28 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="1">
         <v>21</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -989,7 +1007,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1001,7 +1019,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1013,7 +1031,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1025,7 +1043,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1037,7 +1055,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1049,7 +1067,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1061,7 +1079,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1073,7 +1091,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1085,7 +1103,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1097,7 +1115,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>1</v>
       </c>
@@ -1123,21 +1141,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="1">
         <v>1</v>
       </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="E35" s="1">
+        <v>4</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="H35" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1157,7 +1182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1177,7 +1202,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1197,7 +1222,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1217,7 +1242,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1237,7 +1262,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1257,7 +1282,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1277,7 +1302,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1297,7 +1322,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1317,7 +1342,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1337,7 +1362,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1357,7 +1382,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1377,7 +1402,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>

</xml_diff>

<commit_message>
Add yaml settings capability
</commit_message>
<xml_diff>
--- a/fpga/pt_feedback/docs/pt_feedback_addresses.xlsx
+++ b/fpga/pt_feedback/docs/pt_feedback_addresses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/polybox/ETHZ/Programming/Python/rp_interface/fpga/pt_feedback/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A50094-F0CF-6E47-91AF-831567F1EE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4550C35F-55A0-B840-B462-17EF3AD56780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6316E74E-F60B-2E49-B41A-03A0EDA0FE20}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="57">
   <si>
     <t>GPIO Number</t>
   </si>
@@ -199,10 +199,13 @@
     <t>pre-amp</t>
   </si>
   <si>
-    <t>new</t>
-  </si>
-  <si>
     <t>trig mode</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>dds_compiler</t>
   </si>
 </sst>
 </file>
@@ -609,7 +612,7 @@
   <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="I26" sqref="I26:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,7 +881,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -894,7 +897,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -910,7 +913,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -926,7 +929,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -942,7 +945,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -958,7 +961,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -974,7 +977,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -985,17 +988,14 @@
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="I23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1007,7 +1007,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1019,43 +1019,61 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="2">
         <v>24</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="E26" s="2">
+        <v>26</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="2">
         <v>25</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="E27" s="2">
+        <v>25</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="2">
         <v>26</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="E28" s="2">
+        <v>2</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1067,7 +1085,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1079,7 +1097,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1091,7 +1109,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>

</xml_diff>